<commit_message>
Save files using the new Office version
</commit_message>
<xml_diff>
--- a/ERS_proj/KernLWU.xlsx
+++ b/ERS_proj/KernLWU.xlsx
@@ -1,10 +1,16 @@
 
 <file path=xl/workbook.xml><?xml version="1.0" encoding="utf-8"?>
-<workbook xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships">
-  <fileVersion appName="xl" lastEdited="5" lowestEdited="5" rupBuild="9302"/>
+<workbook xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr6="http://schemas.microsoft.com/office/spreadsheetml/2016/revision6" xmlns:xr10="http://schemas.microsoft.com/office/spreadsheetml/2016/revision10" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" mc:Ignorable="x15 xr xr6 xr10 xr2">
+  <fileVersion appName="xl" lastEdited="7" lowestEdited="5" rupBuild="21425"/>
   <workbookPr defaultThemeVersion="124226"/>
+  <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
+    <mc:Choice Requires="x15">
+      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="F:\UCDAVIS\C2VSIM_FG_OR\C2Vsim_FG_v2\ERS_proj\"/>
+    </mc:Choice>
+  </mc:AlternateContent>
+  <xr:revisionPtr revIDLastSave="0" documentId="8_{5567E0C4-C207-48F3-ADC2-BD5CCA6D9569}" xr6:coauthVersionLast="43" xr6:coauthVersionMax="43" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
-    <workbookView xWindow="120" yWindow="75" windowWidth="26835" windowHeight="8775"/>
+    <workbookView xWindow="-120" yWindow="-120" windowWidth="29040" windowHeight="15840" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
   </bookViews>
   <sheets>
     <sheet name="KernLWU" sheetId="1" r:id="rId1"/>
@@ -241,7 +247,7 @@
 </file>
 
 <file path=xl/styles.xml><?xml version="1.0" encoding="utf-8"?>
-<styleSheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
+<styleSheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:x16r2="http://schemas.microsoft.com/office/spreadsheetml/2015/02/main" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" mc:Ignorable="x14ac x16r2 xr">
   <fonts count="18" x14ac:knownFonts="1">
     <font>
       <sz val="11"/>
@@ -774,6 +780,9 @@
     <ext xmlns:x14="http://schemas.microsoft.com/office/spreadsheetml/2009/9/main" uri="{EB79DEF2-80B8-43e5-95BD-54CBDDF9020C}">
       <x14:slicerStyles defaultSlicerStyle="SlicerStyleLight1"/>
     </ext>
+    <ext xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" uri="{9260A510-F301-46a8-8635-F512D64BE5F5}">
+      <x15:timelineStyles defaultTimelineStyle="TimeSlicerStyleLight1"/>
+    </ext>
   </extLst>
 </styleSheet>
 </file>
@@ -821,7 +830,7 @@
     </a:clrScheme>
     <a:fontScheme name="Office">
       <a:majorFont>
-        <a:latin typeface="Cambria"/>
+        <a:latin typeface="Cambria" panose="020F0302020204030204"/>
         <a:ea typeface=""/>
         <a:cs typeface=""/>
         <a:font script="Jpan" typeface="ＭＳ Ｐゴシック"/>
@@ -854,9 +863,26 @@
         <a:font script="Viet" typeface="Times New Roman"/>
         <a:font script="Uigh" typeface="Microsoft Uighur"/>
         <a:font script="Geor" typeface="Sylfaen"/>
+        <a:font script="Armn" typeface="Arial"/>
+        <a:font script="Bugi" typeface="Leelawadee UI"/>
+        <a:font script="Bopo" typeface="Microsoft JhengHei"/>
+        <a:font script="Java" typeface="Javanese Text"/>
+        <a:font script="Lisu" typeface="Segoe UI"/>
+        <a:font script="Mymr" typeface="Myanmar Text"/>
+        <a:font script="Nkoo" typeface="Ebrima"/>
+        <a:font script="Olck" typeface="Nirmala UI"/>
+        <a:font script="Osma" typeface="Ebrima"/>
+        <a:font script="Phag" typeface="Phagspa"/>
+        <a:font script="Syrn" typeface="Estrangelo Edessa"/>
+        <a:font script="Syrj" typeface="Estrangelo Edessa"/>
+        <a:font script="Syre" typeface="Estrangelo Edessa"/>
+        <a:font script="Sora" typeface="Nirmala UI"/>
+        <a:font script="Tale" typeface="Microsoft Tai Le"/>
+        <a:font script="Talu" typeface="Microsoft New Tai Lue"/>
+        <a:font script="Tfng" typeface="Ebrima"/>
       </a:majorFont>
       <a:minorFont>
-        <a:latin typeface="Calibri"/>
+        <a:latin typeface="Calibri" panose="020F0502020204030204"/>
         <a:ea typeface=""/>
         <a:cs typeface=""/>
         <a:font script="Jpan" typeface="ＭＳ Ｐゴシック"/>
@@ -889,6 +915,23 @@
         <a:font script="Viet" typeface="Arial"/>
         <a:font script="Uigh" typeface="Microsoft Uighur"/>
         <a:font script="Geor" typeface="Sylfaen"/>
+        <a:font script="Armn" typeface="Arial"/>
+        <a:font script="Bugi" typeface="Leelawadee UI"/>
+        <a:font script="Bopo" typeface="Microsoft JhengHei"/>
+        <a:font script="Java" typeface="Javanese Text"/>
+        <a:font script="Lisu" typeface="Segoe UI"/>
+        <a:font script="Mymr" typeface="Myanmar Text"/>
+        <a:font script="Nkoo" typeface="Ebrima"/>
+        <a:font script="Olck" typeface="Nirmala UI"/>
+        <a:font script="Osma" typeface="Ebrima"/>
+        <a:font script="Phag" typeface="Phagspa"/>
+        <a:font script="Syrn" typeface="Estrangelo Edessa"/>
+        <a:font script="Syrj" typeface="Estrangelo Edessa"/>
+        <a:font script="Syre" typeface="Estrangelo Edessa"/>
+        <a:font script="Sora" typeface="Nirmala UI"/>
+        <a:font script="Tale" typeface="Microsoft Tai Le"/>
+        <a:font script="Talu" typeface="Microsoft New Tai Lue"/>
+        <a:font script="Tfng" typeface="Ebrima"/>
       </a:minorFont>
     </a:fontScheme>
     <a:fmtScheme name="Office">
@@ -1064,10 +1107,12 @@
 </file>
 
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
-<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
+<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{00000000-0001-0000-0000-000000000000}">
   <dimension ref="A1:AN35"/>
   <sheetViews>
-    <sheetView tabSelected="1" workbookViewId="0"/>
+    <sheetView tabSelected="1" workbookViewId="0">
+      <selection activeCell="A4" sqref="A4"/>
+    </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
   <sheetData>

</xml_diff>